<commit_message>
Signed-off-by: Philip Filippenko <philip.filippenko@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/Assets/Extra/Assignment 1.xlsx
+++ b/Assets/Extra/Assignment 1.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StudentPhilipFilippe\My project\Assets\Extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philip\Desktop\CGnew\Assets\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F35BC6-2B82-4C5C-B31A-085B5B097372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75458CC-6713-4AFD-AD82-636F6C5AAEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment generation" sheetId="1" r:id="rId1"/>
     <sheet name="Map of Assignment" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -525,30 +523,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -579,22 +577,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>201706</xdr:rowOff>
+      <xdr:colOff>721178</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>258536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>776386</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1640182</xdr:rowOff>
+      <xdr:colOff>351361</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4535858</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C443CF35-4AE0-4DC9-801B-A9718B044E23}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE609B39-187B-2A8E-C3E6-D868ED462131}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -610,8 +608,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2386853" y="6017559"/>
-          <a:ext cx="2715004" cy="1438476"/>
+          <a:off x="2558142" y="585107"/>
+          <a:ext cx="2133898" cy="4277322"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -623,22 +621,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>557893</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>394607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1036813</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1725707</xdr:rowOff>
+      <xdr:colOff>759656</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1280556</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76A3737C-B25E-4F39-81CF-1B38D7A82DB8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5982C48-B9FF-C219-8FC3-A454BFD7710F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -654,8 +652,228 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1815353" y="313766"/>
-          <a:ext cx="3546931" cy="1725706"/>
+          <a:off x="2394857" y="6245678"/>
+          <a:ext cx="2705478" cy="885949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>299357</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>340178</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>929804</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4674658</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BC9B8A2-6D71-A565-3626-3892733A1BAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2136321" y="8368392"/>
+          <a:ext cx="3134162" cy="4334480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1102179</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2464444</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1060126</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C239AE4C-85CF-BD62-DBB9-3ED3344C2E31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2939143" y="13688786"/>
+          <a:ext cx="1362265" cy="924054"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1020536</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>312964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>164876</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>4647444</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D9D1923-9FFD-EB66-49A1-EEFA613D4648}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2857500" y="15376071"/>
+          <a:ext cx="1648055" cy="4334480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>993322</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>217714</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>51925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1132242</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8696D92F-3195-A92D-4775-F744F6CE9CCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2830286" y="20805321"/>
+          <a:ext cx="1562318" cy="914528"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>335025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>4725006</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A797C635-2EEA-8391-41BD-AC9DEA0D0425}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2598964" y="22655893"/>
+          <a:ext cx="2076740" cy="4344006"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -956,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1183,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:E15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1208,10 +1426,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="38"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1223,7 +1441,7 @@
     <row r="3" spans="3:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
       <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="6"/>
       <c r="G3" s="11"/>
       <c r="H3" s="7"/>
@@ -1243,10 +1461,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="44"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -1256,7 +1474,7 @@
     <row r="6" spans="3:13" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
       <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1276,10 +1494,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1290,7 +1508,7 @@
     <row r="9" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
       <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
       <c r="H9" s="15"/>
@@ -1310,16 +1528,16 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="40"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
@@ -1327,11 +1545,11 @@
     <row r="12" spans="3:13" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
       <c r="D12" s="35"/>
-      <c r="E12" s="36"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="35"/>
-      <c r="I12" s="36"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1351,10 +1569,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="38"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1367,7 +1585,7 @@
     <row r="15" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
       <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1391,10 +1609,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1407,7 +1625,7 @@
     <row r="18" spans="1:13" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
       <c r="D18" s="35"/>
-      <c r="E18" s="36"/>
+      <c r="E18" s="37"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1428,18 +1646,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="41" t="s">
+      <c r="E20" s="44"/>
+      <c r="F20" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="39" t="s">
+      <c r="G20" s="40"/>
+      <c r="H20" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="40"/>
+      <c r="I20" s="42"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -1448,11 +1666,11 @@
     <row r="21" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
       <c r="D21" s="35"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="42"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="40"/>
       <c r="H21" s="35"/>
-      <c r="I21" s="36"/>
+      <c r="I21" s="37"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -1470,25 +1688,25 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="38"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="39" t="s">
+      <c r="L23" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="M23" s="40"/>
+      <c r="M23" s="42"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
       <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -1496,7 +1714,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
       <c r="L24" s="35"/>
-      <c r="M24" s="36"/>
+      <c r="M24" s="37"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -1509,10 +1727,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="39" t="s">
+      <c r="D26" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="40"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -1524,7 +1742,7 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="35"/>
-      <c r="E27" s="36"/>
+      <c r="E27" s="37"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -1542,15 +1760,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="40"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="38"/>
+      <c r="E29" s="44"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1562,10 +1780,10 @@
     </row>
     <row r="30" spans="1:13" ht="322.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="35"/>
-      <c r="B30" s="36"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="25"/>
       <c r="D30" s="35"/>
-      <c r="E30" s="36"/>
+      <c r="E30" s="37"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1583,44 +1801,44 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="38"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="41" t="s">
+      <c r="E32" s="44"/>
+      <c r="F32" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="37" t="s">
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="38"/>
+      <c r="M32" s="44"/>
     </row>
     <row r="33" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="45"/>
-      <c r="B33" s="43"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="17"/>
       <c r="D33" s="35"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="42"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="40"/>
       <c r="L33" s="35"/>
-      <c r="M33" s="43"/>
+      <c r="M33" s="36"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -1632,46 +1850,33 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
-      <c r="D35" s="39" t="s">
+      <c r="D35" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="40"/>
+      <c r="E35" s="42"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" ht="213.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
       <c r="D36" s="35"/>
-      <c r="E36" s="36"/>
+      <c r="E36" s="37"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
       <c r="H38" s="35"/>
-      <c r="I38" s="43"/>
+      <c r="I38" s="36"/>
     </row>
     <row r="91" ht="0.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H11:I11"/>
@@ -1688,46 +1893,30 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DB12A5-2734-4A80-B355-23ECE7ADE458}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA4FA80-9370-4F95-8930-41199F5C753B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Signed-off-by: Student Philip Filippenko (TL_KCOMP_B_Y3) <t00259086@mymtu.ie>
</commit_message>
<xml_diff>
--- a/Assets/Extra/Assignment 1.xlsx
+++ b/Assets/Extra/Assignment 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philip\Desktop\CGnew\Assets\Extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StudentPhilipFilippe\Desktop\cgnew\Assets\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75458CC-6713-4AFD-AD82-636F6C5AAEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B37B2C-9B87-420B-9F68-1766D617EDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>z = -1</t>
   </si>
@@ -413,7 +413,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -523,34 +523,43 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -577,15 +586,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>721178</xdr:colOff>
+      <xdr:colOff>666749</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>258536</xdr:rowOff>
+      <xdr:rowOff>54428</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>351361</xdr:colOff>
+      <xdr:colOff>1265464</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>4535858</xdr:rowOff>
+      <xdr:rowOff>5100310</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -608,8 +617,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2558142" y="585107"/>
-          <a:ext cx="2133898" cy="4277322"/>
+          <a:off x="2503713" y="380999"/>
+          <a:ext cx="2517322" cy="5045882"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -621,15 +630,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>557893</xdr:colOff>
+      <xdr:colOff>176893</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>394607</xdr:rowOff>
+      <xdr:rowOff>299357</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>759656</xdr:colOff>
+      <xdr:colOff>1665632</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1280556</xdr:rowOff>
+      <xdr:rowOff>1415143</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -652,8 +661,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2394857" y="6245678"/>
-          <a:ext cx="2705478" cy="885949"/>
+          <a:off x="2013857" y="6150428"/>
+          <a:ext cx="3407346" cy="1115786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -671,7 +680,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>929804</xdr:colOff>
+      <xdr:colOff>1514912</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>4674658</xdr:rowOff>
     </xdr:to>
@@ -709,15 +718,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1102179</xdr:colOff>
+      <xdr:colOff>1238250</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>136072</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2464444</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>782208</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1060126</xdr:rowOff>
+      <xdr:rowOff>1087340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -740,52 +749,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2939143" y="13688786"/>
-          <a:ext cx="1362265" cy="924054"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1020536</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>312964</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>164876</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>4647444</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D9D1923-9FFD-EB66-49A1-EEFA613D4648}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2857500" y="15376071"/>
-          <a:ext cx="1648055" cy="4334480"/>
+          <a:off x="3075214" y="13647964"/>
+          <a:ext cx="1462565" cy="992090"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -803,7 +768,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>51925</xdr:colOff>
+      <xdr:colOff>637033</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>1132242</xdr:rowOff>
     </xdr:to>
@@ -821,7 +786,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -841,22 +806,66 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>381000</xdr:rowOff>
+      <xdr:rowOff>204108</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>335025</xdr:colOff>
+      <xdr:colOff>1646465</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>4725006</xdr:rowOff>
+      <xdr:rowOff>5001045</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A797C635-2EEA-8391-41BD-AC9DEA0D0425}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBC9A2FB-BE9B-C191-6A73-E2FDDDFC27B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2122714" y="22479001"/>
+          <a:ext cx="3279322" cy="4796937"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>517071</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>421822</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1532573</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>4765828</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6985DFEE-AF6D-393E-A8FD-B16738281E11}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -872,8 +881,360 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2598964" y="22655893"/>
-          <a:ext cx="2076740" cy="4344006"/>
+          <a:off x="2354035" y="15484929"/>
+          <a:ext cx="2934109" cy="4344006"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>149678</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>680357</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1046518</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06D3D212-88E3-A597-B54F-000BC27AA46A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8341178" y="13675178"/>
+          <a:ext cx="2449286" cy="924054"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>449037</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>353785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1469572</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>4648724</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{153CC5EE-F7E3-0D1F-7926-D587A383A882}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9960430" y="22628678"/>
+          <a:ext cx="2939142" cy="4294939"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>258535</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1559827</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1095501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{432225B9-7EF1-9813-0129-CF72C027EFAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2095499" y="27989893"/>
+          <a:ext cx="3219899" cy="905001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>312965</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1646465</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>5098068</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{306932F1-8094-9EB7-40AD-7BBCE4CF12F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2149929" y="29718000"/>
+          <a:ext cx="3252107" cy="4948389"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>721179</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1537607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1393734</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>2480714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD6203E6-F12E-DF83-65B3-ACEA4054408E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2558143" y="36630428"/>
+          <a:ext cx="2591162" cy="943107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>163285</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1769420</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>4620230</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69E51951-A0B3-886E-839A-348C3A37B5BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2000249" y="39800893"/>
+          <a:ext cx="3524742" cy="4334480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>136071</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>656337</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1034263</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C219DFD-8B0D-B001-4220-5F7D7C364E4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14341928" y="27976286"/>
+          <a:ext cx="3391373" cy="857370"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>217714</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>326572</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>766559</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>4661052</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D80C409D-1387-B393-4889-A55F4B0BE268}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14423571" y="39841715"/>
+          <a:ext cx="3419952" cy="4334480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1175,7 +1536,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1401,19 +1762,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:G21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="4" max="9" width="28.7109375" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="3.7109375" customWidth="1"/>
     <col min="12" max="12" width="43.140625" customWidth="1"/>
@@ -1426,10 +1782,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="44"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1441,7 +1797,7 @@
     <row r="3" spans="3:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
       <c r="D3" s="35"/>
-      <c r="E3" s="37"/>
+      <c r="E3" s="36"/>
       <c r="F3" s="6"/>
       <c r="G3" s="11"/>
       <c r="H3" s="7"/>
@@ -1461,10 +1817,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -1474,7 +1830,7 @@
     <row r="6" spans="3:13" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
       <c r="D6" s="35"/>
-      <c r="E6" s="37"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1494,10 +1850,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="44"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1508,7 +1864,7 @@
     <row r="9" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
       <c r="D9" s="35"/>
-      <c r="E9" s="37"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
       <c r="H9" s="15"/>
@@ -1528,16 +1884,16 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="42"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
@@ -1545,11 +1901,11 @@
     <row r="12" spans="3:13" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
       <c r="D12" s="35"/>
-      <c r="E12" s="37"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="35"/>
-      <c r="I12" s="37"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1569,10 +1925,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="44"/>
+      <c r="E14" s="38"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1585,7 +1941,7 @@
     <row r="15" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
       <c r="D15" s="35"/>
-      <c r="E15" s="37"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1609,10 +1965,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="44"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1625,7 +1981,7 @@
     <row r="18" spans="1:13" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
       <c r="D18" s="35"/>
-      <c r="E18" s="37"/>
+      <c r="E18" s="36"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1646,18 +2002,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="44"/>
-      <c r="F20" s="38" t="s">
+      <c r="E20" s="38"/>
+      <c r="F20" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41" t="s">
+      <c r="G20" s="42"/>
+      <c r="H20" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="42"/>
+      <c r="I20" s="40"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -1666,11 +2022,11 @@
     <row r="21" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
       <c r="D21" s="35"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="40"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="35"/>
-      <c r="I21" s="37"/>
+      <c r="I21" s="36"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -1688,25 +2044,25 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="43" t="s">
+      <c r="D23" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="44"/>
+      <c r="E23" s="38"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="41" t="s">
+      <c r="L23" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="M23" s="42"/>
+      <c r="M23" s="40"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
       <c r="D24" s="35"/>
-      <c r="E24" s="37"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -1714,7 +2070,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
       <c r="L24" s="35"/>
-      <c r="M24" s="37"/>
+      <c r="M24" s="36"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -1727,10 +2083,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="41" t="s">
+      <c r="D26" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="42"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -1742,7 +2098,7 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="35"/>
-      <c r="E27" s="37"/>
+      <c r="E27" s="36"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -1760,15 +2116,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="42"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="44"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1780,10 +2136,10 @@
     </row>
     <row r="30" spans="1:13" ht="322.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="35"/>
-      <c r="B30" s="37"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="25"/>
       <c r="D30" s="35"/>
-      <c r="E30" s="37"/>
+      <c r="E30" s="36"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1801,44 +2157,42 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="43" t="s">
+      <c r="B32" s="38"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="44"/>
-      <c r="F32" s="38" t="s">
+      <c r="E32" s="38"/>
+      <c r="F32" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="43" t="s">
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="44"/>
+      <c r="M32" s="38"/>
     </row>
     <row r="33" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="45"/>
-      <c r="B33" s="36"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="17"/>
       <c r="D33" s="35"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="40"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="42"/>
       <c r="L33" s="35"/>
-      <c r="M33" s="36"/>
+      <c r="M33" s="43"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -1850,33 +2204,54 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
-      <c r="D35" s="41" t="s">
+      <c r="D35" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="42"/>
+      <c r="E35" s="40"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" ht="213.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
       <c r="D36" s="35"/>
-      <c r="E36" s="37"/>
+      <c r="E36" s="36"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="36"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="47"/>
+    </row>
+    <row r="39" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+    </row>
+    <row r="40" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
     </row>
     <row r="91" ht="0.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H11:I11"/>
@@ -1893,25 +2268,12 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>